<commit_message>
fw: add led state pin to ioc
</commit_message>
<xml_diff>
--- a/Hardware/calcolo partitori.xlsx
+++ b/Hardware/calcolo partitori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Desktop/Step-Motor-Test-Bench/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B5A248D-6E0B-E447-8474-E2BACF090FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12CD1FD-7E7F-144A-867F-04EC6F81BD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-18500" windowWidth="26180" windowHeight="10460" xr2:uid="{072F4B72-3FF7-D641-BAAE-6B32E250A867}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{072F4B72-3FF7-D641-BAAE-6B32E250A867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Dispositivo</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>12 -&gt; 5</t>
+  </si>
+  <si>
+    <t>Regolatore</t>
+  </si>
+  <si>
+    <t>Vo = Vref*(1+r2/r1)</t>
+  </si>
+  <si>
+    <t>vref</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>vo</t>
+  </si>
+  <si>
+    <t>r2/r1</t>
+  </si>
+  <si>
+    <t>vo/vref -1</t>
   </si>
 </sst>
 </file>
@@ -485,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A124C48-114A-D549-828A-63C638E66421}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +778,55 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1.25</v>
+      </c>
+      <c r="D17">
+        <f>4.7+3.9</f>
+        <v>8.6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>D17/E17</f>
+        <v>8.6</v>
+      </c>
+      <c r="G17">
+        <f>B17/C17 - 1</f>
+        <v>8.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>